<commit_message>
Fischers Fritze frisst frischen Fisch
</commit_message>
<xml_diff>
--- a/E5 Programmierung/Messaufgabe3.xlsx
+++ b/E5 Programmierung/Messaufgabe3.xlsx
@@ -8,19 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muell\Documents\7_Studium\4_Viertes_Semester\B04_Physik_Grundpraktikum\E5 Gleichrichterschaltungen\E5 Programmierung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D3F088E8-047F-4E17-A72F-89BF2842D9C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB318B9-308C-484A-B12E-DDD79ED18070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10390" yWindow="70" windowWidth="11300" windowHeight="10630" xr2:uid="{5D897228-0EC1-4AE3-9749-5B4EA53B0DCB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{5D897228-0EC1-4AE3-9749-5B4EA53B0DCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Messaufgabe3" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Namensstruktur: Spannungsmessung_EinwegOderZweiweggleichrichtung_MitOderOhneKondensator_Gleichspannungsdrehspulmessinstrument(GDSM)OderWechselspannungdrehspulmessinstrument(WDSM)</t>
   </si>
@@ -52,16 +63,19 @@
     <t>U_2Weg_mitC_WDSM</t>
   </si>
   <si>
-    <t>Quellspannung_vor_Trafo</t>
-  </si>
-  <si>
-    <t>Quellspannung_nach_Trafo</t>
-  </si>
-  <si>
     <t>Unsicherheit im Scheitelwert dU_m in V</t>
   </si>
   <si>
     <t>Unsicherheit (Gleichspannung) dU in Volt</t>
+  </si>
+  <si>
+    <t>Quellspannung_oben_Steckbrett</t>
+  </si>
+  <si>
+    <t>Quellspannung_unten_Steckbrett</t>
+  </si>
+  <si>
+    <t>U_2Weg_ohneC_WDSM</t>
   </si>
 </sst>
 </file>
@@ -905,7 +919,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -930,10 +944,10 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -941,18 +955,19 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <f>26/10</f>
+        <v>2.6</v>
       </c>
       <c r="C4">
         <f>PI()*B4</f>
-        <v>3.1415926535897931</v>
+        <v>8.1681408993334621</v>
       </c>
       <c r="D4">
-        <v>0.01</v>
+        <v>0.5</v>
       </c>
       <c r="E4">
         <f>PI()*D4</f>
-        <v>3.1415926535897934E-2</v>
+        <v>1.5707963267948966</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -960,18 +975,19 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <f>2.6/10</f>
+        <v>0.26</v>
       </c>
       <c r="C5">
         <f>B5</f>
-        <v>1</v>
+        <v>0.26</v>
       </c>
       <c r="D5">
-        <v>0.01</v>
+        <v>0.5</v>
       </c>
       <c r="E5">
         <f>D5</f>
-        <v>0.01</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -979,18 +995,19 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <f>9.5</f>
+        <v>9.5</v>
       </c>
       <c r="C6">
         <f>2*SQRT(2)*B6</f>
-        <v>2.8284271247461903</v>
+        <v>26.870057685088806</v>
       </c>
       <c r="D6">
-        <v>0.01</v>
+        <v>0.5</v>
       </c>
       <c r="E6">
         <f>2*SQRT(2)*D6</f>
-        <v>2.8284271247461905E-2</v>
+        <v>1.4142135623730951</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -998,18 +1015,18 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>10.3</v>
       </c>
       <c r="C7">
         <f>B7</f>
-        <v>1</v>
+        <v>10.3</v>
       </c>
       <c r="D7">
-        <v>0.01</v>
+        <v>0.5</v>
       </c>
       <c r="E7">
         <f>D7</f>
-        <v>0.01</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -1017,37 +1034,39 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <f>61.5/10</f>
+        <v>6.15</v>
       </c>
       <c r="C8">
         <f>PI()/2*B8</f>
-        <v>1.5707963267948966</v>
+        <v>9.6603974097886152</v>
       </c>
       <c r="D8">
-        <v>0.01</v>
+        <v>0.5</v>
       </c>
       <c r="E8">
         <f>PI()/2*D8</f>
-        <v>1.5707963267948967E-2</v>
+        <v>0.78539816339744828</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <f>63.5/10</f>
+        <v>6.35</v>
       </c>
       <c r="C9">
         <f>B9</f>
-        <v>1</v>
+        <v>6.35</v>
       </c>
       <c r="D9">
-        <v>0.01</v>
+        <v>0.5</v>
       </c>
       <c r="E9">
         <f>D9</f>
-        <v>0.01</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -1055,18 +1074,18 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <f>SQRT(2)*B10</f>
-        <v>1.4142135623730951</v>
+        <v>14.142135623730951</v>
       </c>
       <c r="D10">
-        <v>0.01</v>
+        <v>0.5</v>
       </c>
       <c r="E10">
         <f>SQRT(2)*D10</f>
-        <v>1.4142135623730952E-2</v>
+        <v>0.70710678118654757</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -1074,28 +1093,36 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>10.3</v>
       </c>
       <c r="C11">
         <f>B11</f>
-        <v>1</v>
+        <v>10.3</v>
       </c>
       <c r="D11">
-        <v>0.01</v>
+        <v>0.5</v>
       </c>
       <c r="E11">
         <f>D11</f>
-        <v>0.01</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <f>7.1*30</f>
+        <v>213</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <f>7.5*30</f>
+        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>